<commit_message>
Forgot to connect DAC common-mode, easy hardware fix tho
</commit_message>
<xml_diff>
--- a/pcb/icyradio.xlsx
+++ b/pcb/icyradio.xlsx
@@ -300,7 +300,7 @@
     <t>5.62K Ohms</t>
   </si>
   <si>
-    <t>50 Ohms</t>
+    <t>49.9 Ohms</t>
   </si>
   <si>
     <t>510 Ohms</t>
@@ -536,10 +536,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -559,97 +559,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -673,6 +590,89 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -680,15 +680,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -738,7 +738,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,121 +900,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -876,49 +918,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1110,7 +1110,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1130,17 +1141,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1152,6 +1152,30 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1174,32 +1198,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1208,142 +1208,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1353,11 +1353,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1738,8 +1735,8 @@
   <sheetPr/>
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.2" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -1748,1730 +1745,1730 @@
     <col min="2" max="4" width="28.6" customWidth="1"/>
     <col min="5" max="5" width="8.3" customWidth="1"/>
     <col min="6" max="6" width="21.9" customWidth="1"/>
-    <col min="7" max="16384" width="7.2" style="2"/>
+    <col min="7" max="16384" width="7.2" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" spans="1:6">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:6">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>1206</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:6">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="13"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:6">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>10</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="13"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:6">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="13"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:6">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="13"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:6">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="13"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:6">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:6">
-      <c r="A9" s="7">
-        <v>1</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="13"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:6">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>5</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:6">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>17</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:6">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>106</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:6">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>5</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:6">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>9</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:6">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>5</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="13"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:6">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>4</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:6">
-      <c r="A17" s="7">
-        <v>1</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="6">
+        <v>1</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="13"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="1:6">
-      <c r="A18" s="7">
-        <v>1</v>
-      </c>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="6">
+        <v>1</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="13"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:6">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>3</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="13"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="1:6">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>2</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="13" t="s">
+      <c r="E20" s="7"/>
+      <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" spans="1:6">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>2</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="13"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:6">
-      <c r="A22" s="7">
-        <v>1</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="6">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="13"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="12"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:6">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>15</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="13"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="12"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="1:6">
-      <c r="A24" s="7">
-        <v>1</v>
-      </c>
-      <c r="B24" s="8" t="s">
+      <c r="A24" s="6">
+        <v>1</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="13"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="1:6">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>2</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="13"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" s="1" customFormat="1" spans="1:6">
-      <c r="A26" s="7">
+      <c r="A26" s="6">
         <v>2</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="13"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" s="1" customFormat="1" spans="1:6">
-      <c r="A27" s="7">
-        <v>1</v>
-      </c>
-      <c r="B27" s="8" t="s">
+      <c r="A27" s="6">
+        <v>1</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="13"/>
+      <c r="F27" s="12"/>
     </row>
     <row r="28" s="1" customFormat="1" spans="1:6">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>2</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="13"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" s="1" customFormat="1" spans="1:6">
-      <c r="A29" s="7">
-        <v>1</v>
-      </c>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="6">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="13"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30" s="1" customFormat="1" spans="1:6">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>4</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="13"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="31" s="1" customFormat="1" spans="1:6">
-      <c r="A31" s="7">
-        <v>1</v>
-      </c>
-      <c r="B31" s="8" t="s">
+      <c r="A31" s="6">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="13"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" s="1" customFormat="1" spans="1:6">
-      <c r="A32" s="7">
+      <c r="A32" s="6">
         <v>8</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="13"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="12"/>
     </row>
     <row r="33" s="1" customFormat="1" spans="1:6">
-      <c r="A33" s="7">
-        <v>1</v>
-      </c>
-      <c r="B33" s="8" t="s">
+      <c r="A33" s="6">
+        <v>1</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="13"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" s="1" customFormat="1" spans="1:6">
-      <c r="A34" s="7">
+      <c r="A34" s="6">
         <v>4</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="13"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" s="1" customFormat="1" spans="1:6">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>6</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="13"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" s="1" customFormat="1" spans="1:6">
-      <c r="A36" s="7">
+      <c r="A36" s="6">
         <v>2</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="13"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" s="1" customFormat="1" spans="1:6">
-      <c r="A37" s="7">
-        <v>1</v>
-      </c>
-      <c r="B37" s="8" t="s">
+      <c r="A37" s="6">
+        <v>1</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="13"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="12"/>
     </row>
     <row r="38" s="1" customFormat="1" spans="1:6">
-      <c r="A38" s="7">
+      <c r="A38" s="6">
         <v>4</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="13"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="12"/>
     </row>
     <row r="39" s="1" customFormat="1" spans="1:6">
-      <c r="A39" s="7">
-        <v>1</v>
-      </c>
-      <c r="B39" s="8" t="s">
+      <c r="A39" s="6">
+        <v>1</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="13"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="12"/>
     </row>
     <row r="40" s="1" customFormat="1" spans="1:6">
-      <c r="A40" s="7">
+      <c r="A40" s="6">
         <v>2</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="13"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="12"/>
     </row>
     <row r="41" s="1" customFormat="1" spans="1:6">
-      <c r="A41" s="7">
-        <v>1</v>
-      </c>
-      <c r="B41" s="8" t="s">
+      <c r="A41" s="6">
+        <v>1</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="13"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="12"/>
     </row>
     <row r="42" s="1" customFormat="1" spans="1:6">
-      <c r="A42" s="7">
+      <c r="A42" s="6">
         <v>2</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="13"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="12"/>
     </row>
     <row r="43" s="1" customFormat="1" spans="1:6">
-      <c r="A43" s="7">
-        <v>1</v>
-      </c>
-      <c r="B43" s="8" t="s">
+      <c r="A43" s="6">
+        <v>1</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F43" s="13"/>
+      <c r="F43" s="12"/>
     </row>
     <row r="44" s="1" customFormat="1" spans="1:6">
-      <c r="A44" s="7">
+      <c r="A44" s="6">
         <v>6</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="13"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="12"/>
     </row>
     <row r="45" s="1" customFormat="1" spans="1:6">
-      <c r="A45" s="7">
+      <c r="A45" s="6">
         <v>2</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="13"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="12"/>
     </row>
     <row r="46" s="1" customFormat="1" spans="1:6">
-      <c r="A46" s="7">
-        <v>1</v>
-      </c>
-      <c r="B46" s="8" t="s">
+      <c r="A46" s="6">
+        <v>1</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="13" t="s">
+      <c r="E46" s="7"/>
+      <c r="F46" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="1" spans="1:6">
-      <c r="A47" s="7">
-        <v>1</v>
-      </c>
-      <c r="B47" s="8" t="s">
+      <c r="A47" s="6">
+        <v>1</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="13" t="s">
+      <c r="E47" s="7"/>
+      <c r="F47" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="1" spans="1:6">
-      <c r="A48" s="7">
-        <v>1</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="A48" s="6">
+        <v>1</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="13"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="12"/>
     </row>
     <row r="49" s="1" customFormat="1" spans="1:6">
-      <c r="A49" s="7">
-        <v>1</v>
-      </c>
-      <c r="B49" s="8" t="s">
+      <c r="A49" s="6">
+        <v>1</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="13"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="12"/>
     </row>
     <row r="50" s="1" customFormat="1" spans="1:6">
-      <c r="A50" s="7">
+      <c r="A50" s="6">
         <v>10</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="13"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="12"/>
     </row>
     <row r="51" s="1" customFormat="1" spans="1:6">
-      <c r="A51" s="7">
+      <c r="A51" s="6">
         <v>11</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="13"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="12"/>
     </row>
     <row r="52" s="1" customFormat="1" spans="1:6">
-      <c r="A52" s="7">
+      <c r="A52" s="6">
         <v>2</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="13" t="s">
+      <c r="E52" s="7"/>
+      <c r="F52" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="53" s="1" customFormat="1" spans="1:6">
-      <c r="A53" s="7">
-        <v>1</v>
-      </c>
-      <c r="B53" s="8" t="s">
+      <c r="A53" s="6">
+        <v>1</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="8"/>
-      <c r="F53" s="13"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="12"/>
     </row>
     <row r="54" s="1" customFormat="1" spans="1:6">
-      <c r="A54" s="7">
+      <c r="A54" s="6">
         <v>3</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="13"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="12"/>
     </row>
     <row r="55" s="1" customFormat="1" spans="1:6">
-      <c r="A55" s="7">
-        <v>1</v>
-      </c>
-      <c r="B55" s="8" t="s">
+      <c r="A55" s="6">
+        <v>1</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E55" s="8"/>
-      <c r="F55" s="13"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="12"/>
     </row>
     <row r="56" s="1" customFormat="1" spans="1:6">
-      <c r="A56" s="7">
+      <c r="A56" s="6">
         <v>5</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E56" s="8"/>
-      <c r="F56" s="13"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="12"/>
     </row>
     <row r="57" s="1" customFormat="1" spans="1:6">
-      <c r="A57" s="7">
-        <v>1</v>
-      </c>
-      <c r="B57" s="8" t="s">
+      <c r="A57" s="6">
+        <v>1</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="8"/>
-      <c r="F57" s="13"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="12"/>
     </row>
     <row r="58" s="1" customFormat="1" spans="1:6">
-      <c r="A58" s="7">
+      <c r="A58" s="6">
         <v>4</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="8"/>
-      <c r="F58" s="13"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="12"/>
     </row>
     <row r="59" s="1" customFormat="1" spans="1:6">
-      <c r="A59" s="7">
+      <c r="A59" s="6">
         <v>3</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="13"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="12"/>
     </row>
     <row r="60" s="1" customFormat="1" spans="1:6">
-      <c r="A60" s="7">
-        <v>1</v>
-      </c>
-      <c r="B60" s="8" t="s">
+      <c r="A60" s="6">
+        <v>1</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E60" s="8"/>
-      <c r="F60" s="13"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="12"/>
     </row>
     <row r="61" s="1" customFormat="1" spans="1:6">
-      <c r="A61" s="7">
+      <c r="A61" s="6">
         <v>6</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E61" s="8"/>
-      <c r="F61" s="13"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="12"/>
     </row>
     <row r="62" s="1" customFormat="1" spans="1:6">
-      <c r="A62" s="7">
+      <c r="A62" s="6">
         <v>4</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E62" s="8"/>
-      <c r="F62" s="13"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="12"/>
     </row>
     <row r="63" s="1" customFormat="1" spans="1:6">
-      <c r="A63" s="7">
-        <v>1</v>
-      </c>
-      <c r="B63" s="8" t="s">
+      <c r="A63" s="6">
+        <v>1</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D63" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E63" s="8"/>
-      <c r="F63" s="13"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="12"/>
     </row>
     <row r="64" s="1" customFormat="1" spans="1:6">
-      <c r="A64" s="7">
-        <v>1</v>
-      </c>
-      <c r="B64" s="8" t="s">
+      <c r="A64" s="6">
+        <v>1</v>
+      </c>
+      <c r="B64" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D64" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="8"/>
-      <c r="F64" s="13"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="12"/>
     </row>
     <row r="65" s="1" customFormat="1" spans="1:6">
-      <c r="A65" s="7">
-        <v>1</v>
-      </c>
-      <c r="B65" s="8" t="s">
+      <c r="A65" s="6">
+        <v>1</v>
+      </c>
+      <c r="B65" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D65" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E65" s="8"/>
-      <c r="F65" s="13"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="12"/>
     </row>
     <row r="66" s="1" customFormat="1" spans="1:6">
-      <c r="A66" s="7">
-        <v>1</v>
-      </c>
-      <c r="B66" s="8" t="s">
+      <c r="A66" s="6">
+        <v>1</v>
+      </c>
+      <c r="B66" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E66" s="8"/>
-      <c r="F66" s="13"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="12"/>
     </row>
     <row r="67" s="1" customFormat="1" spans="1:6">
-      <c r="A67" s="7">
-        <v>1</v>
-      </c>
-      <c r="B67" s="8" t="s">
+      <c r="A67" s="6">
+        <v>1</v>
+      </c>
+      <c r="B67" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="D67" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E67" s="8"/>
-      <c r="F67" s="13" t="s">
+      <c r="E67" s="7"/>
+      <c r="F67" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="68" s="1" customFormat="1" spans="1:6">
-      <c r="A68" s="7">
-        <v>1</v>
-      </c>
-      <c r="B68" s="8" t="s">
+      <c r="A68" s="6">
+        <v>1</v>
+      </c>
+      <c r="B68" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="D68" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E68" s="8"/>
-      <c r="F68" s="13"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="12"/>
     </row>
     <row r="69" s="1" customFormat="1" spans="1:6">
-      <c r="A69" s="7">
-        <v>1</v>
-      </c>
-      <c r="B69" s="8" t="s">
+      <c r="A69" s="6">
+        <v>1</v>
+      </c>
+      <c r="B69" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="D69" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="13"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="12"/>
     </row>
     <row r="70" s="1" customFormat="1" spans="1:6">
-      <c r="A70" s="7">
-        <v>1</v>
-      </c>
-      <c r="B70" s="8" t="s">
+      <c r="A70" s="6">
+        <v>1</v>
+      </c>
+      <c r="B70" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="13"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="12"/>
     </row>
     <row r="71" s="1" customFormat="1" spans="1:6">
-      <c r="A71" s="7">
-        <v>1</v>
-      </c>
-      <c r="B71" s="8" t="s">
+      <c r="A71" s="6">
+        <v>1</v>
+      </c>
+      <c r="B71" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E71" s="8"/>
-      <c r="F71" s="13"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="12"/>
     </row>
     <row r="72" s="1" customFormat="1" spans="1:6">
-      <c r="A72" s="7">
-        <v>1</v>
-      </c>
-      <c r="B72" s="8" t="s">
+      <c r="A72" s="6">
+        <v>1</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="D72" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E72" s="8"/>
-      <c r="F72" s="13"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="12"/>
     </row>
     <row r="73" s="1" customFormat="1" spans="1:6">
-      <c r="A73" s="7">
-        <v>1</v>
-      </c>
-      <c r="B73" s="8" t="s">
+      <c r="A73" s="6">
+        <v>1</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E73" s="8"/>
-      <c r="F73" s="13"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="12"/>
     </row>
     <row r="74" s="1" customFormat="1" spans="1:6">
-      <c r="A74" s="7">
-        <v>1</v>
-      </c>
-      <c r="B74" s="8" t="s">
+      <c r="A74" s="6">
+        <v>1</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E74" s="8"/>
-      <c r="F74" s="13"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="12"/>
     </row>
     <row r="75" s="1" customFormat="1" spans="1:6">
-      <c r="A75" s="7">
+      <c r="A75" s="6">
         <v>2</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E75" s="8"/>
-      <c r="F75" s="13"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="12"/>
     </row>
     <row r="76" s="1" customFormat="1" spans="1:6">
-      <c r="A76" s="7">
-        <v>1</v>
-      </c>
-      <c r="B76" s="8" t="s">
+      <c r="A76" s="6">
+        <v>1</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D76" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E76" s="8"/>
-      <c r="F76" s="13"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="12"/>
     </row>
     <row r="77" s="1" customFormat="1" spans="1:6">
-      <c r="A77" s="7">
-        <v>1</v>
-      </c>
-      <c r="B77" s="8" t="s">
+      <c r="A77" s="6">
+        <v>1</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D77" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E77" s="8" t="s">
+      <c r="E77" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="13"/>
+      <c r="F77" s="12"/>
     </row>
     <row r="78" s="1" customFormat="1" spans="1:6">
-      <c r="A78" s="7">
-        <v>1</v>
-      </c>
-      <c r="B78" s="8" t="s">
+      <c r="A78" s="6">
+        <v>1</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C78" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E78" s="8"/>
-      <c r="F78" s="13"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="12"/>
     </row>
     <row r="79" s="1" customFormat="1" spans="1:6">
-      <c r="A79" s="15">
+      <c r="A79" s="14">
         <v>5</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="C79" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D79" s="16" t="s">
+      <c r="D79" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E79" s="16"/>
-      <c r="F79" s="19"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="18"/>
     </row>
     <row r="80" s="1" customFormat="1" spans="1:6">
-      <c r="A80" s="7">
+      <c r="A80" s="6">
         <v>2</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E80" s="8" t="s">
+      <c r="E80" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="F80" s="13"/>
+      <c r="F80" s="12"/>
     </row>
     <row r="81" s="1" customFormat="1" spans="1:6">
-      <c r="A81" s="15">
+      <c r="A81" s="14">
         <v>4</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C81" s="16" t="s">
+      <c r="C81" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D81" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E81" s="16"/>
-      <c r="F81" s="19"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="18"/>
     </row>
     <row r="82" s="1" customFormat="1" spans="1:6">
-      <c r="A82" s="7">
+      <c r="A82" s="6">
         <v>2</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C82" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D82" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E82" s="8"/>
-      <c r="F82" s="13"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="12"/>
     </row>
     <row r="83" s="1" customFormat="1" spans="1:6">
-      <c r="A83" s="7">
-        <v>1</v>
-      </c>
-      <c r="B83" s="8" t="s">
+      <c r="A83" s="6">
+        <v>1</v>
+      </c>
+      <c r="B83" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C83" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D83" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E83" s="8"/>
-      <c r="F83" s="13"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="12"/>
     </row>
     <row r="84" s="1" customFormat="1" spans="1:6">
-      <c r="A84" s="7">
-        <v>1</v>
-      </c>
-      <c r="B84" s="8" t="s">
+      <c r="A84" s="6">
+        <v>1</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C84" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="D84" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E84" s="8"/>
-      <c r="F84" s="13"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="12"/>
     </row>
     <row r="85" s="1" customFormat="1" spans="1:6">
-      <c r="A85" s="7">
-        <v>1</v>
-      </c>
-      <c r="B85" s="8" t="s">
+      <c r="A85" s="6">
+        <v>1</v>
+      </c>
+      <c r="B85" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C85" s="8" t="s">
+      <c r="C85" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="D85" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E85" s="8"/>
-      <c r="F85" s="13"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="12"/>
     </row>
     <row r="86" s="1" customFormat="1" spans="1:6">
-      <c r="A86" s="7">
-        <v>1</v>
-      </c>
-      <c r="B86" s="8" t="s">
+      <c r="A86" s="6">
+        <v>1</v>
+      </c>
+      <c r="B86" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C86" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="D86" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E86" s="8"/>
-      <c r="F86" s="13"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="12"/>
     </row>
     <row r="87" s="1" customFormat="1" spans="1:6">
-      <c r="A87" s="7">
-        <v>1</v>
-      </c>
-      <c r="B87" s="8" t="s">
+      <c r="A87" s="6">
+        <v>1</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C87" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D87" s="8" t="s">
+      <c r="D87" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E87" s="8"/>
-      <c r="F87" s="13"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="12"/>
     </row>
     <row r="88" s="1" customFormat="1" spans="1:6">
-      <c r="A88" s="7">
-        <v>1</v>
-      </c>
-      <c r="B88" s="8" t="s">
+      <c r="A88" s="6">
+        <v>1</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D88" s="8" t="s">
+      <c r="D88" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E88" s="8"/>
-      <c r="F88" s="13"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="12"/>
     </row>
     <row r="89" s="1" customFormat="1" spans="1:6">
-      <c r="A89" s="7">
+      <c r="A89" s="6">
         <v>6</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D89" s="8">
+      <c r="D89" s="7">
         <v>603</v>
       </c>
-      <c r="E89" s="8"/>
-      <c r="F89" s="13"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="12"/>
     </row>
     <row r="90" s="1" customFormat="1" spans="1:6">
-      <c r="A90" s="7">
-        <v>1</v>
-      </c>
-      <c r="B90" s="8" t="s">
+      <c r="A90" s="6">
+        <v>1</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C90" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D90" s="8" t="s">
+      <c r="D90" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E90" s="8"/>
-      <c r="F90" s="13"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="12"/>
     </row>
     <row r="91" s="1" customFormat="1" spans="1:6">
-      <c r="A91" s="7">
-        <v>1</v>
-      </c>
-      <c r="B91" s="8" t="s">
+      <c r="A91" s="6">
+        <v>1</v>
+      </c>
+      <c r="B91" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C91" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D91" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E91" s="8"/>
-      <c r="F91" s="13"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="12"/>
     </row>
     <row r="92" s="1" customFormat="1" spans="1:6">
-      <c r="A92" s="7">
-        <v>1</v>
-      </c>
-      <c r="B92" s="8" t="s">
+      <c r="A92" s="6">
+        <v>1</v>
+      </c>
+      <c r="B92" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C92" s="8" t="s">
+      <c r="C92" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D92" s="8" t="s">
+      <c r="D92" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E92" s="8"/>
-      <c r="F92" s="13"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="12"/>
     </row>
     <row r="93" s="1" customFormat="1" spans="1:6">
-      <c r="A93" s="7">
-        <v>1</v>
-      </c>
-      <c r="B93" s="8" t="s">
+      <c r="A93" s="6">
+        <v>1</v>
+      </c>
+      <c r="B93" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C93" s="8" t="s">
+      <c r="C93" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D93" s="8" t="s">
+      <c r="D93" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E93" s="8"/>
-      <c r="F93" s="13"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="12"/>
     </row>
     <row r="94" s="1" customFormat="1" spans="1:6">
-      <c r="A94" s="7">
+      <c r="A94" s="6">
         <v>2</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B94" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C94" s="8" t="s">
+      <c r="C94" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D94" s="8" t="s">
+      <c r="D94" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E94" s="8"/>
-      <c r="F94" s="13"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="12"/>
     </row>
     <row r="95" s="1" customFormat="1" spans="1:6">
-      <c r="A95" s="7">
+      <c r="A95" s="6">
         <v>2</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C95" s="8" t="s">
+      <c r="C95" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D95" s="8" t="s">
+      <c r="D95" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E95" s="8"/>
-      <c r="F95" s="13"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="12"/>
     </row>
     <row r="96" s="1" customFormat="1" spans="1:6">
-      <c r="A96" s="7">
-        <v>1</v>
-      </c>
-      <c r="B96" s="8" t="s">
+      <c r="A96" s="6">
+        <v>1</v>
+      </c>
+      <c r="B96" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C96" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D96" s="8" t="s">
+      <c r="D96" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E96" s="8"/>
-      <c r="F96" s="13"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="12"/>
     </row>
     <row r="97" s="1" customFormat="1" spans="1:6">
-      <c r="A97" s="7">
-        <v>1</v>
-      </c>
-      <c r="B97" s="8" t="s">
+      <c r="A97" s="6">
+        <v>1</v>
+      </c>
+      <c r="B97" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C97" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D97" s="8">
+      <c r="D97" s="7">
         <v>5050</v>
       </c>
-      <c r="E97" s="8"/>
-      <c r="F97" s="13"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="12"/>
     </row>
     <row r="98" s="1" customFormat="1" spans="1:6">
-      <c r="A98" s="7">
-        <v>1</v>
-      </c>
-      <c r="B98" s="8" t="s">
+      <c r="A98" s="6">
+        <v>1</v>
+      </c>
+      <c r="B98" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C98" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D98" s="8" t="s">
+      <c r="D98" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E98" s="8"/>
-      <c r="F98" s="13"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="12"/>
     </row>
     <row r="99" s="1" customFormat="1" spans="1:6">
-      <c r="A99" s="7">
-        <v>1</v>
-      </c>
-      <c r="B99" s="8" t="s">
+      <c r="A99" s="6">
+        <v>1</v>
+      </c>
+      <c r="B99" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C99" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D99" s="8" t="s">
+      <c r="D99" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E99" s="8"/>
-      <c r="F99" s="13"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="12"/>
     </row>
     <row r="100" s="1" customFormat="1" spans="1:6">
-      <c r="A100" s="7">
+      <c r="A100" s="6">
         <v>2</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="C100" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D100" s="8" t="s">
+      <c r="D100" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E100" s="8"/>
-      <c r="F100" s="13"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="12"/>
     </row>
     <row r="101" s="1" customFormat="1" spans="1:6">
-      <c r="A101" s="7">
-        <v>1</v>
-      </c>
-      <c r="B101" s="8" t="s">
+      <c r="A101" s="6">
+        <v>1</v>
+      </c>
+      <c r="B101" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C101" s="8" t="s">
+      <c r="C101" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D101" s="8" t="s">
+      <c r="D101" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E101" s="8"/>
-      <c r="F101" s="13"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="12"/>
     </row>
     <row r="102" s="1" customFormat="1" spans="1:6">
-      <c r="A102" s="7">
+      <c r="A102" s="6">
         <v>2</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C102" s="8" t="s">
+      <c r="C102" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D102" s="8" t="s">
+      <c r="D102" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E102" s="8"/>
-      <c r="F102" s="13"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="12"/>
     </row>
     <row r="103" s="1" customFormat="1" spans="1:6">
-      <c r="A103" s="7">
+      <c r="A103" s="6">
         <v>3</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="B103" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C103" s="8" t="s">
+      <c r="C103" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D103" s="8" t="s">
+      <c r="D103" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E103" s="8"/>
-      <c r="F103" s="13"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="12"/>
     </row>
     <row r="104" s="1" customFormat="1" spans="1:6">
-      <c r="A104" s="7">
+      <c r="A104" s="6">
         <v>3</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C104" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D104" s="8" t="s">
+      <c r="D104" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="E104" s="8" t="s">
+      <c r="E104" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="F104" s="13"/>
+      <c r="F104" s="12"/>
     </row>
     <row r="105" s="1" customFormat="1" spans="1:6">
-      <c r="A105" s="7">
-        <v>1</v>
-      </c>
-      <c r="B105" s="8" t="s">
+      <c r="A105" s="6">
+        <v>1</v>
+      </c>
+      <c r="B105" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="C105" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="D105" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E105" s="8"/>
-      <c r="F105" s="13"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="12"/>
     </row>
     <row r="106" s="1" customFormat="1" ht="16.5" spans="1:6">
-      <c r="A106" s="17">
+      <c r="A106" s="16">
         <v>2</v>
       </c>
-      <c r="B106" s="18" t="s">
+      <c r="B106" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="C106" s="18" t="s">
+      <c r="C106" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="D106" s="18" t="s">
+      <c r="D106" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="E106" s="18"/>
-      <c r="F106" s="20"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>